<commit_message>
spaghetti plot graphical updates
</commit_message>
<xml_diff>
--- a/data/hgb_hct_variants.xlsx
+++ b/data/hgb_hct_variants.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikbao/Documents/GitHub/ery-final/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{6CF35C85-6E76-E045-8EC1-C4BCF94171C1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4F39C434-6E15-7948-84DC-C8E701599105}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="3020" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="3060" yWindow="3020" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hgb_hct_variants" sheetId="1" r:id="rId1"/>
@@ -298,7 +298,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1139,11 +1139,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2868,7 +2868,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1"/>
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>